<commit_message>
now with article titles
</commit_message>
<xml_diff>
--- a/CWBRexport.xlsx
+++ b/CWBRexport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5598,7 +5598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="S306" sqref="S306"/>
     </sheetView>
   </sheetViews>
@@ -27259,10 +27259,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27598,7 +27601,8 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="56" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>